<commit_message>
update excel file: KG(a) --> KG_a
</commit_message>
<xml_diff>
--- a/dataset_parameter_list.xlsx
+++ b/dataset_parameter_list.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\STAT\01_Post\Grobe\awel_decarb_monitoring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\B105P05\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="312" windowWidth="18612" windowHeight="8880" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="315" windowWidth="18615" windowHeight="8880" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="2" r:id="rId1"/>
@@ -85,9 +85,6 @@
     <t>DATA_SOURCE</t>
   </si>
   <si>
-    <t>KG(a)</t>
-  </si>
-  <si>
     <t>Treibhausgas-Fussabdruck</t>
   </si>
   <si>
@@ -368,6 +365,9 @@
   </si>
   <si>
     <t>WHICH_DATA</t>
+  </si>
+  <si>
+    <t>KG_a</t>
   </si>
 </sst>
 </file>
@@ -677,201 +677,201 @@
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>1</v>
       </c>
       <c r="B7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>88</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>91</v>
-      </c>
-      <c r="B9" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>74</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>67</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>72</v>
-      </c>
-      <c r="B15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>73</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>65</v>
-      </c>
-      <c r="B17" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>81</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>82</v>
-      </c>
-      <c r="B19" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>77</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="B23" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>78</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>79</v>
-      </c>
       <c r="B24" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -887,110 +887,110 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="35.8984375" customWidth="1"/>
+    <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="35.875" customWidth="1"/>
     <col min="6" max="6" width="76.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.19921875" customWidth="1"/>
-    <col min="9" max="9" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.69921875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.69921875" customWidth="1"/>
-    <col min="13" max="13" width="20.19921875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.69921875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="80.69921875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.69921875" customWidth="1"/>
+    <col min="7" max="7" width="27.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.25" customWidth="1"/>
+    <col min="9" max="9" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.75" customWidth="1"/>
+    <col min="13" max="13" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.75" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="80.75" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.75" customWidth="1"/>
     <col min="17" max="17" width="38.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="25.09765625" customWidth="1"/>
-    <col min="19" max="19" width="38.09765625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="38.09765625" customWidth="1"/>
+    <col min="18" max="18" width="25.125" customWidth="1"/>
+    <col min="19" max="19" width="38.125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="38.125" customWidth="1"/>
     <col min="21" max="21" width="14" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="15" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" t="s">
         <v>66</v>
       </c>
-      <c r="M1" t="s">
-        <v>67</v>
-      </c>
       <c r="N1" t="s">
+        <v>71</v>
+      </c>
+      <c r="O1" t="s">
         <v>72</v>
       </c>
-      <c r="O1" t="s">
-        <v>73</v>
-      </c>
       <c r="P1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q1" t="s">
+        <v>80</v>
+      </c>
+      <c r="R1" t="s">
         <v>81</v>
-      </c>
-      <c r="R1" t="s">
-        <v>82</v>
       </c>
       <c r="S1" t="s">
         <v>20</v>
       </c>
       <c r="T1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U1" t="s">
+        <v>76</v>
+      </c>
+      <c r="V1" t="s">
         <v>77</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>78</v>
       </c>
-      <c r="W1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -999,25 +999,25 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
       </c>
       <c r="I2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J2">
         <v>2010</v>
       </c>
       <c r="K2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M2" t="s">
         <v>2</v>
@@ -1032,51 +1032,51 @@
         <v>4</v>
       </c>
       <c r="Q2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S2" t="s">
+        <v>41</v>
+      </c>
+      <c r="T2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>27</v>
       </c>
-      <c r="S2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>28</v>
       </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G3" t="s">
         <v>6</v>
       </c>
       <c r="I3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J3">
         <v>2005</v>
       </c>
       <c r="K3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M3" t="s">
         <v>2</v>
@@ -1085,25 +1085,25 @@
         <v>7</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="P3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="T3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1111,31 +1111,31 @@
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
       </c>
       <c r="I4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M4" t="s">
         <v>2</v>
@@ -1144,69 +1144,69 @@
         <v>9</v>
       </c>
       <c r="O4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S4" t="s">
         <v>19</v>
       </c>
       <c r="T4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="C5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J5" s="3">
         <v>2000</v>
       </c>
       <c r="M5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Q5" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="R5" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1214,19 +1214,19 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" t="s">
         <v>89</v>
-      </c>
-      <c r="G6" t="s">
-        <v>90</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
@@ -1236,39 +1236,39 @@
       </c>
       <c r="Q6" s="3"/>
       <c r="R6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S6" t="s">
         <v>16</v>
       </c>
       <c r="T6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
         <v>35</v>
       </c>
-      <c r="B7" t="s">
-        <v>36</v>
-      </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G7" t="s">
         <v>10</v>
       </c>
       <c r="I7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J7">
         <v>2010</v>
@@ -1286,13 +1286,13 @@
         <v>11</v>
       </c>
       <c r="R7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update parameter list with new indicators
</commit_message>
<xml_diff>
--- a/dataset_parameter_list.xlsx
+++ b/dataset_parameter_list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\B105P05\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\JIDFS\USERS\B105PCG\Documents\Projekte\awel_decarb_monitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="179">
   <si>
     <t>px</t>
   </si>
@@ -368,13 +368,202 @@
   </si>
   <si>
     <t>KG_a</t>
+  </si>
+  <si>
+    <t>G3</t>
+  </si>
+  <si>
+    <t>Spezifischer Energiebedarf für Raumwärme und Warmwasser bei reinen Wohnbauten im Kanton Zürich nach Gebäudealtersklassen</t>
+  </si>
+  <si>
+    <t>Spezifischer Energiebedarf Gebäudepark</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>Anteil fossilfreie Gütertransportfahrzeuge im Fahrzeugbestand</t>
+  </si>
+  <si>
+    <t>Fossilfreier Fahrzeugbestand Güterverkehr</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>Anteil fossilfreie Personenwagen bei Neuzulassungen</t>
+  </si>
+  <si>
+    <t>Fossilfreie Neuzulassungen PKW</t>
+  </si>
+  <si>
+    <t>px-x-1103020200_120</t>
+  </si>
+  <si>
+    <t>M4</t>
+  </si>
+  <si>
+    <t>Durchschnittliche CO₂ Emissionen der Personenwagen</t>
+  </si>
+  <si>
+    <t>https://www.uvek-gis.admin.ch/BFE/ogd/21/</t>
+  </si>
+  <si>
+    <t>M5</t>
+  </si>
+  <si>
+    <t>Anteil fossilfreie Gütertransportfahrzeuge bei Neuzulassungen Lieferwagen</t>
+  </si>
+  <si>
+    <t>Fossilfreie Neuzulassungen Güterverkehr</t>
+  </si>
+  <si>
+    <t>IG1</t>
+  </si>
+  <si>
+    <t>Installierte Leistung fossil betriebener Anlagen grösser 1 MW gemäss Grossfeuerungsdatenbank</t>
+  </si>
+  <si>
+    <t>Feuerungsleistung Grossfeuerungen</t>
+  </si>
+  <si>
+    <t>LF2</t>
+  </si>
+  <si>
+    <t>Abgedeckte Güllelager</t>
+  </si>
+  <si>
+    <t>https://www.web.statistik.zh.ch/awel/decarb_monitoring/</t>
+  </si>
+  <si>
+    <t>G3_data.csv</t>
+  </si>
+  <si>
+    <t>IG1_data.csv</t>
+  </si>
+  <si>
+    <t>LF2_data.csv</t>
+  </si>
+  <si>
+    <t>data_t4.csv</t>
+  </si>
+  <si>
+    <t>Bedarfsjahr</t>
+  </si>
+  <si>
+    <t>Energiebedarf</t>
+  </si>
+  <si>
+    <t>kWh/m2</t>
+  </si>
+  <si>
+    <t>Spezifischer Energiebedarf</t>
+  </si>
+  <si>
+    <t>Benzin, Diesel, Elektrisch, Anderer, ohne Motor</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Anzahl Gütertransportfahrzeuge [Anz.]</t>
+  </si>
+  <si>
+    <t>Benzin, Diesel, Benzin-elektrisch: Normal-Hybrid, Benzin-elektrisch: Plug-in-Hybrid, Diesel-elektrisch: Normal-Hybrid, Diesel-elektrisch: Plug-in-Hybrid, Elektrisch, Wasserstoff, Gas (mono- und bivalent) , Anderer, Ohne Motor</t>
+  </si>
+  <si>
+    <t>Anzahl Neuzulassungen PW [Anz.]</t>
+  </si>
+  <si>
+    <t>Neue Inverkehrsetzungen von Strassenfahrzeugen (IVS), Bundesamt für Strassen (ASTRA) - IVZ-Fahrzeuge</t>
+  </si>
+  <si>
+    <t>ZH, CH</t>
+  </si>
+  <si>
+    <t>Emission</t>
+  </si>
+  <si>
+    <t>date,ZH,BE,LU,UR,SZ,OW,NW,GL,ZG,FR,SO,BS,BL,SH,AR,AI,SG,GR,AG,TG,TI,VD,VS,NE,GE,JU</t>
+  </si>
+  <si>
+    <t>g CO2 / km</t>
+  </si>
+  <si>
+    <t>CO2-Emissionen pro Kilometer</t>
+  </si>
+  <si>
+    <t>Bundesamt für Energie (BFE)</t>
+  </si>
+  <si>
+    <t>total_variable</t>
+  </si>
+  <si>
+    <t>Anzahl Neuzulassungen Gütertransportfahrzeuge [Anz.]</t>
+  </si>
+  <si>
+    <t>Brennstoff</t>
+  </si>
+  <si>
+    <t>Erdgas, Heizöl</t>
+  </si>
+  <si>
+    <t>kW</t>
+  </si>
+  <si>
+    <t>Installierte Feuerungsleistung in kW</t>
+  </si>
+  <si>
+    <t>Anteil_abgedeckt</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Anteil abgedeckte m3 Güllelager (%)</t>
+  </si>
+  <si>
+    <t>DIMENSION1_COL</t>
+  </si>
+  <si>
+    <t>DIMENSION1_ID</t>
+  </si>
+  <si>
+    <t>DIMENSION1_NAME</t>
+  </si>
+  <si>
+    <t>DIMENSION2_COL</t>
+  </si>
+  <si>
+    <t>DIMENSION2_ID</t>
+  </si>
+  <si>
+    <t>DIMENSION2_NAME</t>
+  </si>
+  <si>
+    <t>Fahrzeuggruppe / -art</t>
+  </si>
+  <si>
+    <t>Personenwagen</t>
+  </si>
+  <si>
+    <t>100,200,300,310,400,410,500,550,600,9900,9999</t>
+  </si>
+  <si>
+    <t>Sachentransportfahrzeuge</t>
+  </si>
+  <si>
+    <t>100,200,500,9900,9999</t>
+  </si>
+  <si>
+    <t>opendata</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -398,6 +587,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1D1C1D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -416,10 +619,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -427,8 +631,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -885,10 +1092,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W7"/>
+  <dimension ref="A1:Z14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -902,19 +1109,20 @@
     <col min="10" max="10" width="12.75" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.75" customWidth="1"/>
     <col min="13" max="13" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.75" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="80.75" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.75" customWidth="1"/>
-    <col min="17" max="17" width="38.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="25.125" customWidth="1"/>
-    <col min="19" max="19" width="38.125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="38.125" customWidth="1"/>
-    <col min="21" max="21" width="14" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="20.25" customWidth="1"/>
+    <col min="17" max="17" width="20.75" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="80.75" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.75" customWidth="1"/>
+    <col min="20" max="20" width="38.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="25.125" customWidth="1"/>
+    <col min="22" max="22" width="38.125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="38.125" customWidth="1"/>
+    <col min="24" max="24" width="14" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>70</v>
       </c>
@@ -955,37 +1163,46 @@
         <v>66</v>
       </c>
       <c r="N1" t="s">
-        <v>71</v>
+        <v>167</v>
       </c>
       <c r="O1" t="s">
-        <v>72</v>
+        <v>168</v>
       </c>
       <c r="P1" t="s">
-        <v>64</v>
+        <v>169</v>
       </c>
       <c r="Q1" t="s">
+        <v>170</v>
+      </c>
+      <c r="R1" t="s">
+        <v>171</v>
+      </c>
+      <c r="S1" t="s">
+        <v>172</v>
+      </c>
+      <c r="T1" t="s">
         <v>80</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>81</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>37</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>76</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>77</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1031,20 +1248,20 @@
       <c r="P2" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="T2" t="s">
         <v>43</v>
       </c>
-      <c r="R2" t="s">
+      <c r="U2" t="s">
         <v>26</v>
       </c>
-      <c r="S2" t="s">
+      <c r="V2" t="s">
         <v>41</v>
       </c>
-      <c r="T2" t="s">
+      <c r="W2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1090,20 +1307,20 @@
       <c r="P3" t="s">
         <v>44</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="T3" t="s">
         <v>31</v>
       </c>
-      <c r="R3" t="s">
+      <c r="U3" t="s">
         <v>33</v>
       </c>
-      <c r="S3" t="s">
+      <c r="V3" t="s">
         <v>29</v>
       </c>
-      <c r="T3" t="s">
+      <c r="W3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1149,20 +1366,20 @@
       <c r="P4" t="s">
         <v>45</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="T4" t="s">
         <v>51</v>
       </c>
-      <c r="R4" t="s">
+      <c r="U4" t="s">
         <v>25</v>
       </c>
-      <c r="S4" t="s">
+      <c r="V4" t="s">
         <v>19</v>
       </c>
-      <c r="T4" t="s">
+      <c r="W4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>115</v>
       </c>
@@ -1193,20 +1410,20 @@
       <c r="M5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Q5" s="3" t="s">
+      <c r="T5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="R5" s="3" t="s">
+      <c r="U5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="S5" s="3" t="s">
+      <c r="V5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="T5" s="3" t="s">
+      <c r="W5" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1234,18 +1451,18 @@
       <c r="J6">
         <v>2010</v>
       </c>
-      <c r="Q6" s="3"/>
-      <c r="R6" t="s">
+      <c r="T6" s="3"/>
+      <c r="U6" t="s">
         <v>53</v>
       </c>
-      <c r="S6" t="s">
+      <c r="V6" t="s">
         <v>16</v>
       </c>
-      <c r="T6" t="s">
+      <c r="W6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1282,22 +1499,422 @@
       <c r="P7" t="s">
         <v>7</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="T7" t="s">
         <v>11</v>
       </c>
-      <c r="R7" t="s">
+      <c r="U7" t="s">
         <v>36</v>
       </c>
-      <c r="S7" t="s">
+      <c r="V7" t="s">
         <v>39</v>
       </c>
-      <c r="T7" t="s">
+      <c r="W7" t="s">
         <v>38</v>
       </c>
     </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" t="s">
+        <v>137</v>
+      </c>
+      <c r="G8" t="s">
+        <v>138</v>
+      </c>
+      <c r="I8" t="s">
+        <v>142</v>
+      </c>
+      <c r="J8">
+        <v>1990</v>
+      </c>
+      <c r="N8" t="s">
+        <v>143</v>
+      </c>
+      <c r="P8" t="s">
+        <v>143</v>
+      </c>
+      <c r="T8" t="s">
+        <v>144</v>
+      </c>
+      <c r="U8" t="s">
+        <v>145</v>
+      </c>
+      <c r="V8" t="s">
+        <v>39</v>
+      </c>
+      <c r="W8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" t="s">
+        <v>125</v>
+      </c>
+      <c r="I9" t="s">
+        <v>74</v>
+      </c>
+      <c r="J9">
+        <v>2005</v>
+      </c>
+      <c r="K9" t="s">
+        <v>68</v>
+      </c>
+      <c r="L9" t="s">
+        <v>30</v>
+      </c>
+      <c r="M9" t="s">
+        <v>2</v>
+      </c>
+      <c r="N9" t="s">
+        <v>173</v>
+      </c>
+      <c r="O9">
+        <v>300</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>7</v>
+      </c>
+      <c r="R9" t="s">
+        <v>177</v>
+      </c>
+      <c r="S9" t="s">
+        <v>146</v>
+      </c>
+      <c r="T9" t="s">
+        <v>147</v>
+      </c>
+      <c r="U9" t="s">
+        <v>148</v>
+      </c>
+      <c r="V9" t="s">
+        <v>29</v>
+      </c>
+      <c r="W9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" t="s">
+        <v>125</v>
+      </c>
+      <c r="I10" t="s">
+        <v>74</v>
+      </c>
+      <c r="J10">
+        <v>2005</v>
+      </c>
+      <c r="K10" t="s">
+        <v>68</v>
+      </c>
+      <c r="L10" t="s">
+        <v>30</v>
+      </c>
+      <c r="M10" t="s">
+        <v>2</v>
+      </c>
+      <c r="N10" t="s">
+        <v>173</v>
+      </c>
+      <c r="O10">
+        <v>100</v>
+      </c>
+      <c r="P10" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>7</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="S10" t="s">
+        <v>149</v>
+      </c>
+      <c r="T10" t="s">
+        <v>147</v>
+      </c>
+      <c r="U10" t="s">
+        <v>150</v>
+      </c>
+      <c r="V10" t="s">
+        <v>151</v>
+      </c>
+      <c r="W10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" t="s">
+        <v>178</v>
+      </c>
+      <c r="F11" t="s">
+        <v>128</v>
+      </c>
+      <c r="G11" t="s">
+        <v>141</v>
+      </c>
+      <c r="I11" t="s">
+        <v>74</v>
+      </c>
+      <c r="J11">
+        <v>2014</v>
+      </c>
+      <c r="K11" t="s">
+        <v>152</v>
+      </c>
+      <c r="M11" t="s">
+        <v>2</v>
+      </c>
+      <c r="N11" t="s">
+        <v>153</v>
+      </c>
+      <c r="P11" t="s">
+        <v>154</v>
+      </c>
+      <c r="T11" t="s">
+        <v>155</v>
+      </c>
+      <c r="U11" t="s">
+        <v>156</v>
+      </c>
+      <c r="V11" t="s">
+        <v>157</v>
+      </c>
+      <c r="W11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" t="s">
+        <v>131</v>
+      </c>
+      <c r="D12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" t="s">
+        <v>125</v>
+      </c>
+      <c r="I12" t="s">
+        <v>74</v>
+      </c>
+      <c r="J12">
+        <v>2005</v>
+      </c>
+      <c r="K12" t="s">
+        <v>68</v>
+      </c>
+      <c r="L12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M12" t="s">
+        <v>2</v>
+      </c>
+      <c r="N12" t="s">
+        <v>173</v>
+      </c>
+      <c r="O12">
+        <v>300</v>
+      </c>
+      <c r="P12" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>7</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="S12" t="s">
+        <v>149</v>
+      </c>
+      <c r="T12" t="s">
+        <v>147</v>
+      </c>
+      <c r="U12" t="s">
+        <v>159</v>
+      </c>
+      <c r="V12" t="s">
+        <v>151</v>
+      </c>
+      <c r="W12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C13" t="s">
+        <v>134</v>
+      </c>
+      <c r="D13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="G13" t="s">
+        <v>139</v>
+      </c>
+      <c r="I13" t="s">
+        <v>74</v>
+      </c>
+      <c r="J13">
+        <v>2022</v>
+      </c>
+      <c r="N13" t="s">
+        <v>160</v>
+      </c>
+      <c r="P13" t="s">
+        <v>161</v>
+      </c>
+      <c r="T13" t="s">
+        <v>162</v>
+      </c>
+      <c r="U13" t="s">
+        <v>163</v>
+      </c>
+      <c r="V13" t="s">
+        <v>39</v>
+      </c>
+      <c r="W13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C14" t="s">
+        <v>136</v>
+      </c>
+      <c r="D14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" t="s">
+        <v>137</v>
+      </c>
+      <c r="G14" t="s">
+        <v>140</v>
+      </c>
+      <c r="I14" t="s">
+        <v>74</v>
+      </c>
+      <c r="J14">
+        <v>2022</v>
+      </c>
+      <c r="N14" t="s">
+        <v>164</v>
+      </c>
+      <c r="T14" t="s">
+        <v>165</v>
+      </c>
+      <c r="U14" t="s">
+        <v>166</v>
+      </c>
+      <c r="V14" t="s">
+        <v>39</v>
+      </c>
+      <c r="W14" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F13" r:id="rId1"/>
+    <hyperlink ref="F14" r:id="rId2"/>
+    <hyperlink ref="F8" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;D</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Adding scripts w/ computation and export file for M3 and M5
</commit_message>
<xml_diff>
--- a/dataset_parameter_list.xlsx
+++ b/dataset_parameter_list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="177">
   <si>
     <t>px</t>
   </si>
@@ -97,12 +97,6 @@
     <t>Mio. t CO2-eq</t>
   </si>
   <si>
-    <t>Gebäude [Anz.]</t>
-  </si>
-  <si>
-    <t>Personen [Anz.]</t>
-  </si>
-  <si>
     <t>M1</t>
   </si>
   <si>
@@ -121,9 +115,6 @@
     <t>INDICATOR_NAME</t>
   </si>
   <si>
-    <t>Personenwagen [Anz.]</t>
-  </si>
-  <si>
     <t>M8</t>
   </si>
   <si>
@@ -463,18 +454,9 @@
     <t>Benzin, Diesel, Elektrisch, Anderer, ohne Motor</t>
   </si>
   <si>
-    <t>#</t>
-  </si>
-  <si>
-    <t>Anzahl Gütertransportfahrzeuge [Anz.]</t>
-  </si>
-  <si>
     <t>Benzin, Diesel, Benzin-elektrisch: Normal-Hybrid, Benzin-elektrisch: Plug-in-Hybrid, Diesel-elektrisch: Normal-Hybrid, Diesel-elektrisch: Plug-in-Hybrid, Elektrisch, Wasserstoff, Gas (mono- und bivalent) , Anderer, Ohne Motor</t>
   </si>
   <si>
-    <t>Anzahl Neuzulassungen PW [Anz.]</t>
-  </si>
-  <si>
     <t>Neue Inverkehrsetzungen von Strassenfahrzeugen (IVS), Bundesamt für Strassen (ASTRA) - IVZ-Fahrzeuge</t>
   </si>
   <si>
@@ -499,9 +481,6 @@
     <t>total_variable</t>
   </si>
   <si>
-    <t>Anzahl Neuzulassungen Gütertransportfahrzeuge [Anz.]</t>
-  </si>
-  <si>
     <t>Brennstoff</t>
   </si>
   <si>
@@ -557,13 +536,28 @@
   </si>
   <si>
     <t>opendata</t>
+  </si>
+  <si>
+    <t>Anzahl Neuzulassungen PW</t>
+  </si>
+  <si>
+    <t>Anzahl</t>
+  </si>
+  <si>
+    <t>Anzahl Gütertransportfahrzeuge</t>
+  </si>
+  <si>
+    <t>Anzahl Neuzulassungen Gütertransportfahrzeuge</t>
+  </si>
+  <si>
+    <t>Personen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -586,13 +580,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -619,11 +606,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -631,11 +617,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -891,50 +875,50 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -942,103 +926,103 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B10" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B15" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B18" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B19" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -1046,39 +1030,39 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1095,7 +1079,8 @@
   <dimension ref="A1:Z14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1124,82 +1109,82 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="J1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="K1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="M1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N1" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="O1" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="P1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="Q1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="R1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="S1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="T1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="U1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="V1" t="s">
         <v>20</v>
       </c>
       <c r="W1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="X1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="Y1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="Z1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
@@ -1207,7 +1192,7 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -1216,25 +1201,25 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
       </c>
       <c r="I2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J2">
         <v>2010</v>
       </c>
       <c r="K2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="M2" t="s">
         <v>2</v>
@@ -1249,51 +1234,51 @@
         <v>4</v>
       </c>
       <c r="T2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="U2" t="s">
-        <v>26</v>
+        <v>176</v>
       </c>
       <c r="V2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="W2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G3" t="s">
         <v>6</v>
       </c>
       <c r="I3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J3">
         <v>2005</v>
       </c>
       <c r="K3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M3" t="s">
         <v>2</v>
@@ -1302,22 +1287,22 @@
         <v>7</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="P3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="T3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="U3" t="s">
-        <v>33</v>
+        <v>167</v>
       </c>
       <c r="V3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="W3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
@@ -1328,31 +1313,31 @@
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
       </c>
       <c r="I4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="M4" t="s">
         <v>2</v>
@@ -1361,48 +1346,48 @@
         <v>9</v>
       </c>
       <c r="O4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="P4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="T4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="U4" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="V4" t="s">
         <v>19</v>
       </c>
       <c r="W4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" t="s">
         <v>59</v>
       </c>
-      <c r="E5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F5" t="s">
-        <v>62</v>
-      </c>
       <c r="G5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="J5" s="3">
         <v>2000</v>
@@ -1420,7 +1405,7 @@
         <v>22</v>
       </c>
       <c r="W5" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
@@ -1431,19 +1416,19 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6" t="s">
         <v>85</v>
       </c>
-      <c r="D6" t="s">
-        <v>112</v>
-      </c>
-      <c r="E6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F6" t="s">
-        <v>88</v>
-      </c>
       <c r="G6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
@@ -1453,39 +1438,39 @@
       </c>
       <c r="T6" s="3"/>
       <c r="U6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="V6" t="s">
         <v>16</v>
       </c>
       <c r="W6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" t="s">
         <v>60</v>
-      </c>
-      <c r="E7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F7" t="s">
-        <v>63</v>
       </c>
       <c r="G7" t="s">
         <v>10</v>
       </c>
       <c r="I7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J7">
         <v>2010</v>
@@ -1503,418 +1488,413 @@
         <v>11</v>
       </c>
       <c r="U7" t="s">
+        <v>33</v>
+      </c>
+      <c r="V7" t="s">
         <v>36</v>
       </c>
-      <c r="V7" t="s">
-        <v>39</v>
-      </c>
       <c r="W7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F8" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="I8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="J8">
         <v>1990</v>
       </c>
       <c r="N8" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="P8" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="T8" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="U8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="V8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="W8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D9" t="s">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="I9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J9">
         <v>2005</v>
       </c>
       <c r="K9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M9" t="s">
         <v>2</v>
       </c>
       <c r="N9" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="O9">
         <v>300</v>
       </c>
-      <c r="P9" s="6" t="s">
-        <v>176</v>
+      <c r="P9" s="5" t="s">
+        <v>169</v>
       </c>
       <c r="Q9" t="s">
         <v>7</v>
       </c>
       <c r="R9" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="S9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="T9" t="s">
-        <v>147</v>
+        <v>173</v>
       </c>
       <c r="U9" t="s">
-        <v>148</v>
+        <v>174</v>
       </c>
       <c r="V9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="W9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C10" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D10" t="s">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G10" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="I10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J10">
         <v>2005</v>
       </c>
       <c r="K10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M10" t="s">
         <v>2</v>
       </c>
       <c r="N10" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="O10">
         <v>100</v>
       </c>
       <c r="P10" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="Q10" t="s">
         <v>7</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="S10" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="T10" t="s">
-        <v>147</v>
+        <v>173</v>
       </c>
       <c r="U10" t="s">
-        <v>150</v>
+        <v>172</v>
       </c>
       <c r="V10" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="W10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E11" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="F11" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G11" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="I11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J11">
         <v>2014</v>
       </c>
       <c r="K11" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="M11" t="s">
         <v>2</v>
       </c>
       <c r="N11" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="P11" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="T11" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="U11" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="V11" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="W11" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C12" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D12" t="s">
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G12" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="I12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J12">
         <v>2005</v>
       </c>
       <c r="K12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M12" t="s">
         <v>2</v>
       </c>
       <c r="N12" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="O12">
         <v>300</v>
       </c>
-      <c r="P12" s="6" t="s">
-        <v>176</v>
+      <c r="P12" s="5" t="s">
+        <v>169</v>
       </c>
       <c r="Q12" t="s">
         <v>7</v>
       </c>
       <c r="R12" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="S12" t="s">
+        <v>144</v>
+      </c>
+      <c r="T12" t="s">
+        <v>173</v>
+      </c>
+      <c r="U12" t="s">
         <v>175</v>
       </c>
-      <c r="S12" t="s">
-        <v>149</v>
-      </c>
-      <c r="T12" t="s">
-        <v>147</v>
-      </c>
-      <c r="U12" t="s">
-        <v>159</v>
-      </c>
       <c r="V12" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="W12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C13" t="s">
+        <v>131</v>
+      </c>
+      <c r="D13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" t="s">
         <v>134</v>
       </c>
-      <c r="D13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>137</v>
-      </c>
       <c r="G13" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="I13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J13">
         <v>2022</v>
       </c>
       <c r="N13" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="P13" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="T13" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="U13" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="V13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="W13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C14" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F14" t="s">
+        <v>134</v>
+      </c>
+      <c r="G14" t="s">
         <v>137</v>
       </c>
-      <c r="G14" t="s">
-        <v>140</v>
-      </c>
       <c r="I14" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J14">
         <v>2022</v>
       </c>
       <c r="N14" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="T14" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="U14" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="V14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="W14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F13" r:id="rId1"/>
-    <hyperlink ref="F14" r:id="rId2"/>
-    <hyperlink ref="F8" r:id="rId3"/>
-  </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;D</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
M2 computations (begin) + new parameter file (fixed M2 px path)
</commit_message>
<xml_diff>
--- a/dataset_parameter_list.xlsx
+++ b/dataset_parameter_list.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\JIDFS\USERS\B105PCG\Documents\Projekte\awel_decarb_monitoring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\B105P05\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="315" windowWidth="18615" windowHeight="8880" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26820" windowHeight="10620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="178">
   <si>
     <t>px</t>
   </si>
@@ -551,6 +551,9 @@
   </si>
   <si>
     <t>Personen</t>
+  </si>
+  <si>
+    <t>px-x-1103020100_101</t>
   </si>
 </sst>
 </file>
@@ -1080,7 +1083,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E7" sqref="E7:E8"/>
+      <selection pane="topRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1564,7 +1567,7 @@
         <v>58</v>
       </c>
       <c r="G9" t="s">
-        <v>122</v>
+        <v>177</v>
       </c>
       <c r="I9" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
fix entry for dimension label M2 🐛
</commit_message>
<xml_diff>
--- a/dataset_parameter_list.xlsx
+++ b/dataset_parameter_list.xlsx
@@ -532,9 +532,6 @@
     <t>Sachentransportfahrzeuge</t>
   </si>
   <si>
-    <t>100,200,500,9900,9999</t>
-  </si>
-  <si>
     <t>opendata</t>
   </si>
   <si>
@@ -554,6 +551,9 @@
   </si>
   <si>
     <t>px-x-1103020100_101</t>
+  </si>
+  <si>
+    <t>100,200,300,9900,9999</t>
   </si>
 </sst>
 </file>
@@ -871,12 +871,12 @@
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>44</v>
       </c>
@@ -884,7 +884,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -892,7 +892,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -900,7 +900,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -908,7 +908,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>88</v>
       </c>
@@ -916,7 +916,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -924,7 +924,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -932,7 +932,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>84</v>
       </c>
@@ -940,7 +940,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>87</v>
       </c>
@@ -948,7 +948,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>70</v>
       </c>
@@ -956,7 +956,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -964,7 +964,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>64</v>
       </c>
@@ -972,7 +972,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -980,7 +980,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -988,7 +988,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>68</v>
       </c>
@@ -996,7 +996,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>69</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>61</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>77</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>78</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>73</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>74</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>75</v>
       </c>
@@ -1082,35 +1082,35 @@
   <dimension ref="A1:Z14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G9" sqref="G9"/>
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="35.875" customWidth="1"/>
+    <col min="1" max="1" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="35.8984375" customWidth="1"/>
     <col min="6" max="6" width="76.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.25" customWidth="1"/>
-    <col min="9" max="9" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.75" customWidth="1"/>
-    <col min="13" max="13" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="20.25" customWidth="1"/>
-    <col min="17" max="17" width="20.75" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="80.75" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.75" customWidth="1"/>
+    <col min="7" max="7" width="27.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.19921875" customWidth="1"/>
+    <col min="9" max="9" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.69921875" customWidth="1"/>
+    <col min="13" max="13" width="20.19921875" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="20.19921875" customWidth="1"/>
+    <col min="17" max="17" width="20.69921875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="80.69921875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.69921875" customWidth="1"/>
     <col min="20" max="20" width="38.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="25.125" customWidth="1"/>
-    <col min="22" max="22" width="38.125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="38.125" customWidth="1"/>
+    <col min="21" max="21" width="25.09765625" customWidth="1"/>
+    <col min="22" max="22" width="38.09765625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="38.09765625" customWidth="1"/>
     <col min="24" max="24" width="14" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="15" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>40</v>
       </c>
       <c r="U2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="V2" t="s">
         <v>38</v>
@@ -1249,7 +1249,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>112</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>113</v>
       </c>
@@ -1547,7 +1547,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>116</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>58</v>
       </c>
       <c r="G9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I9" t="s">
         <v>71</v>
@@ -1597,16 +1597,16 @@
         <v>7</v>
       </c>
       <c r="R9" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="S9" t="s">
         <v>143</v>
       </c>
       <c r="T9" t="s">
+        <v>172</v>
+      </c>
+      <c r="U9" t="s">
         <v>173</v>
-      </c>
-      <c r="U9" t="s">
-        <v>174</v>
       </c>
       <c r="V9" t="s">
         <v>27</v>
@@ -1615,7 +1615,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>119</v>
       </c>
@@ -1671,10 +1671,10 @@
         <v>144</v>
       </c>
       <c r="T10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="U10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="V10" t="s">
         <v>145</v>
@@ -1683,7 +1683,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>123</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>57</v>
       </c>
       <c r="E11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F11" t="s">
         <v>125</v>
@@ -1736,7 +1736,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>126</v>
       </c>
@@ -1792,10 +1792,10 @@
         <v>144</v>
       </c>
       <c r="T12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="U12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="V12" t="s">
         <v>145</v>
@@ -1804,7 +1804,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>129</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>132</v>
       </c>

</xml_diff>